<commit_message>
priming update (look at why compareKeys isn't working)
</commit_message>
<xml_diff>
--- a/priming_updated.xlsx
+++ b/priming_updated.xlsx
@@ -1,15 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11013"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="62" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A481BD28-052B-41D7-BDE0-D716F9B39EE6}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bowdoin-my.sharepoint.com/personal/ljanas_bowdoin_edu/Documents/Desktop/PSYC 2740-0/FOOBLY APPLE/foobly-apple-experiment/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="76" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC64B5B1-F5C3-D842-BC9C-73A459A8B151}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="20260" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$J$1:$J$59</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="28">
   <si>
     <t>block_number</t>
   </si>
@@ -121,7 +129,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,12 +145,24 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -157,9 +177,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,25 +516,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J59"/>
+  <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -544,7 +566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75">
+    <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -572,11 +594,14 @@
       <c r="I2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="15.75">
+      <c r="J2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -607,8 +632,11 @@
       <c r="J3" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.75">
+      <c r="K3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -639,8 +667,11 @@
       <c r="J4" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.75">
+      <c r="K4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -671,8 +702,11 @@
       <c r="J5" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75">
+      <c r="K5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -700,11 +734,14 @@
       <c r="I6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15.75">
+      <c r="J6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -735,8 +772,11 @@
       <c r="J7" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="15.75">
+      <c r="K7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -767,8 +807,11 @@
       <c r="J8" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.75">
+      <c r="K8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -799,8 +842,11 @@
       <c r="J9" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="15.75">
+      <c r="K9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -828,11 +874,14 @@
       <c r="I10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="15.75">
+      <c r="J10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -860,11 +909,11 @@
       <c r="I11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15.75">
+      <c r="J11" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -892,11 +941,11 @@
       <c r="I12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15.75">
+      <c r="J12" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -924,11 +973,11 @@
       <c r="I13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15.75">
+      <c r="J13" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -956,11 +1005,11 @@
       <c r="I14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75">
+      <c r="J14" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>1</v>
       </c>
@@ -988,11 +1037,11 @@
       <c r="I15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J15" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="15.75">
+      <c r="J15" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>1</v>
       </c>
@@ -1020,11 +1069,11 @@
       <c r="I16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J16" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="15.75">
+      <c r="J16" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>1</v>
       </c>
@@ -1056,7 +1105,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75">
+    <row r="18" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>1</v>
       </c>
@@ -1088,7 +1137,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75">
+    <row r="19" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>1</v>
       </c>
@@ -1120,7 +1169,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.75">
+    <row r="20" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>1</v>
       </c>
@@ -1152,7 +1201,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75">
+    <row r="21" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>1</v>
       </c>
@@ -1184,7 +1233,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75">
+    <row r="22" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>1</v>
       </c>
@@ -1216,7 +1265,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15.75">
+    <row r="23" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>1</v>
       </c>
@@ -1244,11 +1293,11 @@
       <c r="I23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J23" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="15.75">
+      <c r="J23" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>1</v>
       </c>
@@ -1276,11 +1325,11 @@
       <c r="I24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J24" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="15.75">
+      <c r="J24" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>1</v>
       </c>
@@ -1308,11 +1357,11 @@
       <c r="I25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J25" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="15.75">
+      <c r="J25" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>1</v>
       </c>
@@ -1340,11 +1389,11 @@
       <c r="I26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J26" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="15.75">
+      <c r="J26" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>1</v>
       </c>
@@ -1372,11 +1421,11 @@
       <c r="I27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J27" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="15.75">
+      <c r="J27" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>1</v>
       </c>
@@ -1404,11 +1453,11 @@
       <c r="I28" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J28" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="15.75">
+      <c r="J28" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>1</v>
       </c>
@@ -1440,7 +1489,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15.75">
+    <row r="30" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>1</v>
       </c>
@@ -1472,7 +1521,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15.75">
+    <row r="31" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>1</v>
       </c>
@@ -1504,7 +1553,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="15.75">
+    <row r="32" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>1</v>
       </c>
@@ -1536,7 +1585,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="15.75">
+    <row r="33" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>1</v>
       </c>
@@ -1568,7 +1617,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15.75">
+    <row r="34" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>1</v>
       </c>
@@ -1600,7 +1649,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15.75">
+    <row r="35" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>1</v>
       </c>
@@ -1628,11 +1677,11 @@
       <c r="I35" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J35" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="15.75">
+      <c r="J35" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>1</v>
       </c>
@@ -1660,11 +1709,11 @@
       <c r="I36" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J36" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="15.75">
+      <c r="J36" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>1</v>
       </c>
@@ -1692,11 +1741,11 @@
       <c r="I37" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J37" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="15.75">
+      <c r="J37" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>1</v>
       </c>
@@ -1724,11 +1773,11 @@
       <c r="I38" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J38" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="15.75">
+      <c r="J38" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>1</v>
       </c>
@@ -1756,11 +1805,11 @@
       <c r="I39" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J39" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="15.75">
+      <c r="J39" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>1</v>
       </c>
@@ -1788,11 +1837,11 @@
       <c r="I40" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J40" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="15.75">
+      <c r="J40" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>1</v>
       </c>
@@ -1824,7 +1873,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="15.75">
+    <row r="42" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>1</v>
       </c>
@@ -1856,7 +1905,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="15.75">
+    <row r="43" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>1</v>
       </c>
@@ -1888,7 +1937,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="15.75">
+    <row r="44" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>1</v>
       </c>
@@ -1920,7 +1969,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="15.75">
+    <row r="45" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>1</v>
       </c>
@@ -1952,7 +2001,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="15.75">
+    <row r="46" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>1</v>
       </c>
@@ -1984,7 +2033,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15.75">
+    <row r="47" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>1</v>
       </c>
@@ -2012,11 +2061,11 @@
       <c r="I47" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J47" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="15.75">
+      <c r="J47" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>1</v>
       </c>
@@ -2044,11 +2093,11 @@
       <c r="I48" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J48" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="15.75">
+      <c r="J48" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>1</v>
       </c>
@@ -2076,11 +2125,11 @@
       <c r="I49" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J49" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="15.75">
+      <c r="J49" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>1</v>
       </c>
@@ -2108,11 +2157,11 @@
       <c r="I50" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J50" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="15.75">
+      <c r="J50" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>1</v>
       </c>
@@ -2140,11 +2189,11 @@
       <c r="I51" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J51" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" ht="15.75">
+      <c r="J51" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>1</v>
       </c>
@@ -2172,11 +2221,11 @@
       <c r="I52" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J52" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" ht="15.75">
+      <c r="J52" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>1</v>
       </c>
@@ -2208,7 +2257,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="15.75">
+    <row r="54" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>1</v>
       </c>
@@ -2240,7 +2289,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="15.75">
+    <row r="55" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>1</v>
       </c>
@@ -2272,7 +2321,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="15.75">
+    <row r="56" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>1</v>
       </c>
@@ -2304,7 +2353,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="15.75">
+    <row r="57" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>1</v>
       </c>
@@ -2336,7 +2385,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="15.75">
+    <row r="58" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>1</v>
       </c>
@@ -2368,12 +2417,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="15.75">
+    <row r="59" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B59" s="1">
         <v>2</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="J1:J59" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated prime and added valence_code
</commit_message>
<xml_diff>
--- a/priming_updated.xlsx
+++ b/priming_updated.xlsx
@@ -518,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>